<commit_message>
sarfasl haye dc motor bedoone tartib
</commit_message>
<xml_diff>
--- a/تدریس آردینو.xlsx
+++ b/تدریس آردینو.xlsx
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="788"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="788" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId2"/>
-    <sheet name="5 دکمه" sheetId="9" r:id="rId3"/>
-    <sheet name="4 مقدمه ای بر سریال" sheetId="11" r:id="rId4"/>
-    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId5"/>
-    <sheet name="2 چشمک زن " sheetId="3" r:id="rId6"/>
-    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId7"/>
-    <sheet name="پیش نیاز" sheetId="7" r:id="rId8"/>
-    <sheet name="مدار منطقی" sheetId="8" r:id="rId9"/>
+    <sheet name="سرو" sheetId="14" r:id="rId2"/>
+    <sheet name="موتور دی سی دو" sheetId="13" r:id="rId3"/>
+    <sheet name="موتور دی سی یک" sheetId="12" r:id="rId4"/>
+    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId5"/>
+    <sheet name="5 دکمه" sheetId="9" r:id="rId6"/>
+    <sheet name="4 مقدمه ای بر سریال" sheetId="11" r:id="rId7"/>
+    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId8"/>
+    <sheet name="2 چشمک زن " sheetId="3" r:id="rId9"/>
+    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId10"/>
+    <sheet name="پیش نیاز" sheetId="7" r:id="rId11"/>
+    <sheet name="مدار منطقی" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="182">
   <si>
     <t>معرفی اردینو</t>
   </si>
@@ -298,9 +301,6 @@
     <t>موارد استفاده</t>
   </si>
   <si>
-    <t>مدار تغزیه</t>
-  </si>
-  <si>
     <t>دلیل وجود</t>
   </si>
   <si>
@@ -527,6 +527,60 @@
   </si>
   <si>
     <t>معرفی آردینو</t>
+  </si>
+  <si>
+    <t>موتور دی سی یک</t>
+  </si>
+  <si>
+    <t>موتور دی سی دو</t>
+  </si>
+  <si>
+    <t>مدار تغذیه</t>
+  </si>
+  <si>
+    <t>موتور دی سی چیست</t>
+  </si>
+  <si>
+    <t>روشن کردن موتور</t>
+  </si>
+  <si>
+    <t>Tip 122</t>
+  </si>
+  <si>
+    <t>کنترل یک جهته بدون سرعت</t>
+  </si>
+  <si>
+    <t>کنترل یک جهته با سرعت</t>
+  </si>
+  <si>
+    <t>انواع دی سی</t>
+  </si>
+  <si>
+    <t>نحوه عملکرد براش</t>
+  </si>
+  <si>
+    <t>دیود جریان برگشتی</t>
+  </si>
+  <si>
+    <t>توضیح دوباره جدایی منبع تغذیه از کنترلر</t>
+  </si>
+  <si>
+    <t>پل H</t>
+  </si>
+  <si>
+    <t>IC L298</t>
+  </si>
+  <si>
+    <t>ماژول L298</t>
+  </si>
+  <si>
+    <t>IC L293</t>
+  </si>
+  <si>
+    <t>شیلد L293</t>
+  </si>
+  <si>
+    <t>شیلد L298n</t>
   </si>
 </sst>
 </file>
@@ -883,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -899,7 +953,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -941,7 +995,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -958,7 +1012,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -969,7 +1023,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -1032,6 +1086,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
@@ -1043,6 +1100,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>165</v>
+      </c>
       <c r="C12" t="s">
         <v>32</v>
       </c>
@@ -1054,6 +1114,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
       <c r="C13" t="s">
         <v>35</v>
       </c>
@@ -1115,17 +1178,17 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1133,379 +1196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.625" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E6"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.375" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="31.375" customWidth="1"/>
-    <col min="7" max="7" width="28.125" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.25" customWidth="1"/>
-    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1606,7 +1297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -1623,19 +1314,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
         <v>94</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1643,7 +1334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1658,47 +1349,532 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>104</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>105</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>106</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>107</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>108</v>
-      </c>
-      <c r="I1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A10:D12"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E6"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="31.375" customWidth="1"/>
+    <col min="7" max="7" width="28.125" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
         <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mabahese servo va moarrefi motorha
</commit_message>
<xml_diff>
--- a/تدریس آردینو.xlsx
+++ b/تدریس آردینو.xlsx
@@ -13,17 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="سرو" sheetId="14" r:id="rId2"/>
-    <sheet name="موتور دی سی دو" sheetId="13" r:id="rId3"/>
-    <sheet name="موتور دی سی یک" sheetId="12" r:id="rId4"/>
-    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId5"/>
-    <sheet name="5 دکمه" sheetId="9" r:id="rId6"/>
-    <sheet name="4 مقدمه ای بر سریال" sheetId="11" r:id="rId7"/>
-    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId8"/>
-    <sheet name="2 چشمک زن " sheetId="3" r:id="rId9"/>
-    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId10"/>
-    <sheet name="پیش نیاز" sheetId="7" r:id="rId11"/>
-    <sheet name="مدار منطقی" sheetId="8" r:id="rId12"/>
+    <sheet name="معرفی موتورها" sheetId="15" r:id="rId2"/>
+    <sheet name="سرو" sheetId="14" r:id="rId3"/>
+    <sheet name="موتور دی سی دو" sheetId="13" r:id="rId4"/>
+    <sheet name="موتور دی سی یک" sheetId="12" r:id="rId5"/>
+    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId6"/>
+    <sheet name="5 دکمه" sheetId="9" r:id="rId7"/>
+    <sheet name="4 مقدمه ای بر سریال" sheetId="11" r:id="rId8"/>
+    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId9"/>
+    <sheet name="2 چشمک زن " sheetId="3" r:id="rId10"/>
+    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId11"/>
+    <sheet name="پیش نیاز" sheetId="7" r:id="rId12"/>
+    <sheet name="مدار منطقی" sheetId="8" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="202">
   <si>
     <t>معرفی اردینو</t>
   </si>
@@ -581,6 +582,66 @@
   </si>
   <si>
     <t>شیلد L298n</t>
+  </si>
+  <si>
+    <t>سرو چیست</t>
+  </si>
+  <si>
+    <t>کاربرد</t>
+  </si>
+  <si>
+    <t>ساختار داخلی</t>
+  </si>
+  <si>
+    <t>انواع سرو</t>
+  </si>
+  <si>
+    <t>سرو 180</t>
+  </si>
+  <si>
+    <t>سرو 360</t>
+  </si>
+  <si>
+    <t>کتابخانه سرو</t>
+  </si>
+  <si>
+    <t>توضیح دستورات کتابخانه</t>
+  </si>
+  <si>
+    <t>راه انداختن سرو</t>
+  </si>
+  <si>
+    <t>معرفی موتورها</t>
+  </si>
+  <si>
+    <t>موتور الکتریکی چیست</t>
+  </si>
+  <si>
+    <t>انواع دسته بندی موتورها</t>
+  </si>
+  <si>
+    <t>AC-DC</t>
+  </si>
+  <si>
+    <t>سه فاز - تک فاز</t>
+  </si>
+  <si>
+    <t>دسته بندی بازار</t>
+  </si>
+  <si>
+    <t>براش</t>
+  </si>
+  <si>
+    <t>استپ</t>
+  </si>
+  <si>
+    <t>خصوصیات موتور</t>
+  </si>
+  <si>
+    <t>گشتاور</t>
+  </si>
+  <si>
+    <t>سرعت زاویه</t>
   </si>
 </sst>
 </file>
@@ -1086,9 +1147,6 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>164</v>
-      </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
@@ -1100,9 +1158,6 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>165</v>
-      </c>
       <c r="C12" t="s">
         <v>32</v>
       </c>
@@ -1115,7 +1170,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>191</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
@@ -1128,6 +1183,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>164</v>
+      </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
@@ -1139,6 +1197,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>165</v>
+      </c>
       <c r="C15" t="s">
         <v>41</v>
       </c>
@@ -1150,6 +1211,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
       <c r="C16" t="s">
         <v>44</v>
       </c>
@@ -1197,6 +1261,86 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1297,7 +1441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -1334,7 +1478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1399,17 +1543,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A10:D12"/>
   <sheetViews>
@@ -1455,7 +1704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1510,7 +1759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1583,7 +1832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1663,7 +1912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1717,7 +1966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
@@ -1800,84 +2049,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.25" customWidth="1"/>
-    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sarfaslhaye keypad va tab haye step va brushless
</commit_message>
<xml_diff>
--- a/تدریس آردینو.xlsx
+++ b/تدریس آردینو.xlsx
@@ -9,22 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="788" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="788"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="معرفی موتورها" sheetId="15" r:id="rId2"/>
-    <sheet name="سرو" sheetId="14" r:id="rId3"/>
-    <sheet name="موتور دی سی دو" sheetId="13" r:id="rId4"/>
-    <sheet name="موتور دی سی یک" sheetId="12" r:id="rId5"/>
-    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId6"/>
-    <sheet name="5 دکمه" sheetId="9" r:id="rId7"/>
-    <sheet name="4 مقدمه ای بر سریال" sheetId="11" r:id="rId8"/>
-    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId9"/>
-    <sheet name="2 چشمک زن " sheetId="3" r:id="rId10"/>
-    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId11"/>
-    <sheet name="پیش نیاز" sheetId="7" r:id="rId12"/>
-    <sheet name="مدار منطقی" sheetId="8" r:id="rId13"/>
+    <sheet name="براشلس" sheetId="17" r:id="rId2"/>
+    <sheet name="استپ" sheetId="16" r:id="rId3"/>
+    <sheet name="سرو" sheetId="14" r:id="rId4"/>
+    <sheet name="موتور دی سی دو" sheetId="13" r:id="rId5"/>
+    <sheet name="موتور دی سی یک" sheetId="12" r:id="rId6"/>
+    <sheet name="معرفی موتورها" sheetId="15" r:id="rId7"/>
+    <sheet name="7 کیپد" sheetId="18" r:id="rId8"/>
+    <sheet name="6 انواع متغیر ها" sheetId="10" r:id="rId9"/>
+    <sheet name="5 دکمه" sheetId="9" r:id="rId10"/>
+    <sheet name="4 مقدمه ای بر سریال" sheetId="11" r:id="rId11"/>
+    <sheet name="3 ترانزیستو و رله " sheetId="4" r:id="rId12"/>
+    <sheet name="2 چشمک زن " sheetId="3" r:id="rId13"/>
+    <sheet name="1 معرفی آردینو " sheetId="2" r:id="rId14"/>
+    <sheet name="پیش نیاز" sheetId="7" r:id="rId15"/>
+    <sheet name="مدار منطقی" sheetId="8" r:id="rId16"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="216">
   <si>
     <t>معرفی اردینو</t>
   </si>
@@ -642,6 +645,48 @@
   </si>
   <si>
     <t>سرعت زاویه</t>
+  </si>
+  <si>
+    <t>تنوع بازار</t>
+  </si>
+  <si>
+    <t>کتابخانه چیست</t>
+  </si>
+  <si>
+    <t>نصب کتابخانه</t>
+  </si>
+  <si>
+    <t>از طریق library</t>
+  </si>
+  <si>
+    <t>از طریق ide</t>
+  </si>
+  <si>
+    <t>کتابخانه کیپد</t>
+  </si>
+  <si>
+    <t>تعریف ماتریس</t>
+  </si>
+  <si>
+    <t>تعریف کیپد</t>
+  </si>
+  <si>
+    <t>دستورات کیپد</t>
+  </si>
+  <si>
+    <t>getKey</t>
+  </si>
+  <si>
+    <t>waitForKey</t>
+  </si>
+  <si>
+    <t>setHoldTime</t>
+  </si>
+  <si>
+    <t>setDebounceTime</t>
+  </si>
+  <si>
+    <t>اتصال پین ها</t>
   </si>
 </sst>
 </file>
@@ -998,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1261,6 +1306,225 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E6"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="31.375" customWidth="1"/>
+    <col min="7" max="7" width="28.125" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1340,7 +1604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -1441,7 +1705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -1478,7 +1742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1543,69 +1807,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1658,7 +1882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A10:D12"/>
   <sheetViews>
@@ -1704,7 +1928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1759,7 +1983,146 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1830,223 +2193,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E6"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.375" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="31.375" customWidth="1"/>
-    <col min="7" max="7" width="28.125" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>